<commit_message>
Registro de las habilidades del postulante y implementacoin del modulo de preguntas
</commit_message>
<xml_diff>
--- a/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
+++ b/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angeles Valdospin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSelectAI\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3211B3F1-0232-4453-B4F8-0336A849F019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEB3346-9728-447E-8D35-C909E21FE9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1342,9 +1342,6 @@
     <t>0706191558</t>
   </si>
   <si>
-    <t>0927159111</t>
-  </si>
-  <si>
     <t>0917406837</t>
   </si>
   <si>
@@ -1352,6 +1349,9 @@
   </si>
   <si>
     <t>0925710253</t>
+  </si>
+  <si>
+    <t>1234567890</t>
   </si>
 </sst>
 </file>
@@ -1431,7 +1431,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1743,7 +1743,7 @@
   <dimension ref="A1:I107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4741,7 +4741,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B104" t="s">
         <v>427</v>
@@ -4770,7 +4770,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B105" t="s">
         <v>434</v>
@@ -4799,7 +4799,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B106" t="s">
         <v>430</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B107" t="s">
         <v>436</v>

</xml_diff>

<commit_message>
Se añadio la generacion de preguntas con IA, y se finalizo el modulo de Vacantes. Se completo el login del postulante y la eleccion de habilidades junto al envio de correo y se añadio el token de acceso a las rutas de la entrevista
</commit_message>
<xml_diff>
--- a/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
+++ b/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSelectAI\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEB3346-9728-447E-8D35-C909E21FE9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F9197B-2F35-44CB-825D-4B030D039AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1742,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4736,7 +4736,7 @@
         <v>407</v>
       </c>
       <c r="I103" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Se valido toda la parte de postulante, se añadio verficacion de dispositivo. OJO FALTA EL TEMA DE SEGURIDAD Y DIVIDIR EN MAS COMPONENTES
</commit_message>
<xml_diff>
--- a/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
+++ b/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSelectAI\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A7A14D-DBA4-48C6-9538-2FBBFF6CBE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B3D89A-04BC-4278-8B57-2868C6988B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="347">
   <si>
     <t>Cedula</t>
   </si>
@@ -1052,6 +1052,18 @@
   </si>
   <si>
     <t>Itinerario 1</t>
+  </si>
+  <si>
+    <t>0706191558</t>
+  </si>
+  <si>
+    <t>0796381964</t>
+  </si>
+  <si>
+    <t>0769579066</t>
+  </si>
+  <si>
+    <t>0755590360</t>
   </si>
 </sst>
 </file>
@@ -1110,11 +1122,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1419,23 +1435,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1467,7 +1482,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1371721533</v>
       </c>
       <c r="B2" t="s">
@@ -1499,7 +1514,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>1246093661</v>
       </c>
       <c r="B3" t="s">
@@ -1531,7 +1546,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>1288678217</v>
       </c>
       <c r="B4" t="s">
@@ -1563,7 +1578,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>1222504389</v>
       </c>
       <c r="B5" t="s">
@@ -1595,7 +1610,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>1394915856</v>
       </c>
       <c r="B6" t="s">
@@ -1626,8 +1641,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>2433208844</v>
       </c>
       <c r="B7" t="s">
@@ -1659,7 +1674,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>2480129594</v>
       </c>
       <c r="B8" t="s">
@@ -1691,7 +1706,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>720728941</v>
       </c>
       <c r="B9" t="s">
@@ -1722,8 +1737,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>759287723</v>
       </c>
       <c r="B10" t="s">
@@ -1755,7 +1770,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>948220113</v>
       </c>
       <c r="B11" t="s">
@@ -1787,7 +1802,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>2424328482</v>
       </c>
       <c r="B12" t="s">
@@ -1819,7 +1834,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>981338500</v>
       </c>
       <c r="B13" t="s">
@@ -1851,7 +1866,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>1398772538</v>
       </c>
       <c r="B14" t="s">
@@ -1882,8 +1897,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>783507267</v>
       </c>
       <c r="B15" t="s">
@@ -1914,8 +1929,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>915095024</v>
       </c>
       <c r="B16" t="s">
@@ -1946,8 +1961,8 @@
         <v>342</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>1238089041</v>
       </c>
       <c r="B17" t="s">
@@ -1978,8 +1993,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>2438826166</v>
       </c>
       <c r="B18" t="s">
@@ -2011,7 +2026,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>2437369800</v>
       </c>
       <c r="B19" t="s">
@@ -2043,7 +2058,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>1290513566</v>
       </c>
       <c r="B20" t="s">
@@ -2074,8 +2089,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>1298166873</v>
       </c>
       <c r="B21" t="s">
@@ -2107,7 +2122,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>1208290064</v>
       </c>
       <c r="B22" t="s">
@@ -2138,8 +2153,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>1353558433</v>
       </c>
       <c r="B23" t="s">
@@ -2171,7 +2186,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>2484816966</v>
       </c>
       <c r="B24" t="s">
@@ -2203,7 +2218,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>976268018</v>
       </c>
       <c r="B25" t="s">
@@ -2234,8 +2249,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>1263998831</v>
       </c>
       <c r="B26" t="s">
@@ -2267,7 +2282,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>940382957</v>
       </c>
       <c r="B27" t="s">
@@ -2299,7 +2314,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>1341949434</v>
       </c>
       <c r="B28" t="s">
@@ -2331,7 +2346,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>941235061</v>
       </c>
       <c r="B29" t="s">
@@ -2363,7 +2378,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>1214481323</v>
       </c>
       <c r="B30" t="s">
@@ -2395,7 +2410,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>1356191641</v>
       </c>
       <c r="B31" t="s">
@@ -2427,7 +2442,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>1365912843</v>
       </c>
       <c r="B32" t="s">
@@ -2459,7 +2474,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>1389254132</v>
       </c>
       <c r="B33" t="s">
@@ -2490,8 +2505,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
         <v>1315841607</v>
       </c>
       <c r="B34" t="s">
@@ -2522,8 +2537,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
         <v>913117316</v>
       </c>
       <c r="B35" t="s">
@@ -2555,7 +2570,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>2478878553</v>
       </c>
       <c r="B36" t="s">
@@ -2586,8 +2601,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
         <v>767903179</v>
       </c>
       <c r="B37" t="s">
@@ -2619,7 +2634,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>734405479</v>
       </c>
       <c r="B38" t="s">
@@ -2650,8 +2665,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
         <v>1385081441</v>
       </c>
       <c r="B39" t="s">
@@ -2683,7 +2698,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>1363601483</v>
       </c>
       <c r="B40" t="s">
@@ -2714,8 +2729,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
         <v>970506323</v>
       </c>
       <c r="B41" t="s">
@@ -2747,7 +2762,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="3">
         <v>999254687</v>
       </c>
       <c r="B42" t="s">
@@ -2778,8 +2793,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
         <v>1285055467</v>
       </c>
       <c r="B43" t="s">
@@ -2810,8 +2825,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
         <v>743867233</v>
       </c>
       <c r="B44" t="s">
@@ -2843,7 +2858,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="3">
         <v>1215012383</v>
       </c>
       <c r="B45" t="s">
@@ -2875,7 +2890,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="3">
         <v>707986153</v>
       </c>
       <c r="B46" t="s">
@@ -2907,7 +2922,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="3">
         <v>1382548764</v>
       </c>
       <c r="B47" t="s">
@@ -2939,7 +2954,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="A48" s="3">
         <v>703902643</v>
       </c>
       <c r="B48" t="s">
@@ -2971,7 +2986,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="3">
         <v>932447936</v>
       </c>
       <c r="B49" t="s">
@@ -3003,7 +3018,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="A50" s="3">
         <v>1375016160</v>
       </c>
       <c r="B50" t="s">
@@ -3035,7 +3050,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="3">
         <v>1362721868</v>
       </c>
       <c r="B51" t="s">
@@ -3067,7 +3082,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="A52" s="3">
         <v>1315564515</v>
       </c>
       <c r="B52" t="s">
@@ -3098,8 +3113,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
         <v>720369045</v>
       </c>
       <c r="B53" t="s">
@@ -3131,7 +3146,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="A54" s="3">
         <v>701429329</v>
       </c>
       <c r="B54" t="s">
@@ -3163,7 +3178,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="A55" s="3">
         <v>1369410495</v>
       </c>
       <c r="B55" t="s">
@@ -3195,7 +3210,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="3">
         <v>2490497344</v>
       </c>
       <c r="B56" t="s">
@@ -3227,7 +3242,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="3">
         <v>2470782917</v>
       </c>
       <c r="B57" t="s">
@@ -3259,7 +3274,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="A58" s="3">
         <v>2455004254</v>
       </c>
       <c r="B58" t="s">
@@ -3291,7 +3306,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="A59" s="3">
         <v>1343888050</v>
       </c>
       <c r="B59" t="s">
@@ -3323,7 +3338,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="A60" s="3">
         <v>1307099349</v>
       </c>
       <c r="B60" t="s">
@@ -3355,7 +3370,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="3">
         <v>1269564804</v>
       </c>
       <c r="B61" t="s">
@@ -3387,7 +3402,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="A62" s="3">
         <v>2437859241</v>
       </c>
       <c r="B62" t="s">
@@ -3418,8 +3433,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A63">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
         <v>1322971279</v>
       </c>
       <c r="B63" t="s">
@@ -3450,8 +3465,8 @@
         <v>342</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A64">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
         <v>906071292</v>
       </c>
       <c r="B64" t="s">
@@ -3482,8 +3497,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A65">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
         <v>1213722938</v>
       </c>
       <c r="B65" t="s">
@@ -3514,8 +3529,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A66">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
         <v>1317833324</v>
       </c>
       <c r="B66" t="s">
@@ -3547,7 +3562,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67">
+      <c r="A67" s="3">
         <v>711864590</v>
       </c>
       <c r="B67" t="s">
@@ -3579,7 +3594,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68">
+      <c r="A68" s="3">
         <v>763408693</v>
       </c>
       <c r="B68" t="s">
@@ -3610,8 +3625,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A69">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
         <v>1321145842</v>
       </c>
       <c r="B69" t="s">
@@ -3643,7 +3658,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70">
+      <c r="A70" s="3">
         <v>1366822708</v>
       </c>
       <c r="B70" t="s">
@@ -3675,7 +3690,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71">
+      <c r="A71" s="3">
         <v>1296234117</v>
       </c>
       <c r="B71" t="s">
@@ -3707,7 +3722,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72">
+      <c r="A72" s="3">
         <v>1360531481</v>
       </c>
       <c r="B72" t="s">
@@ -3739,7 +3754,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73">
+      <c r="A73" s="3">
         <v>705926578</v>
       </c>
       <c r="B73" t="s">
@@ -3771,7 +3786,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74">
+      <c r="A74" s="3">
         <v>1391155583</v>
       </c>
       <c r="B74" t="s">
@@ -3803,7 +3818,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75">
+      <c r="A75" s="3">
         <v>1351171567</v>
       </c>
       <c r="B75" t="s">
@@ -3835,7 +3850,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76">
+      <c r="A76" s="3">
         <v>1284151530</v>
       </c>
       <c r="B76" t="s">
@@ -3867,7 +3882,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77">
+      <c r="A77" s="3">
         <v>772589041</v>
       </c>
       <c r="B77" t="s">
@@ -3898,8 +3913,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A78">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
         <v>2475427227</v>
       </c>
       <c r="B78" t="s">
@@ -3931,7 +3946,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79">
+      <c r="A79" s="3">
         <v>1228744778</v>
       </c>
       <c r="B79" t="s">
@@ -3963,8 +3978,8 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>769579066</v>
+      <c r="A80" s="3" t="s">
+        <v>345</v>
       </c>
       <c r="B80" t="s">
         <v>84</v>
@@ -3995,8 +4010,8 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>796381964</v>
+      <c r="A81" s="3" t="s">
+        <v>344</v>
       </c>
       <c r="B81" t="s">
         <v>85</v>
@@ -4027,7 +4042,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82">
+      <c r="A82" s="3">
         <v>2448799579</v>
       </c>
       <c r="B82" t="s">
@@ -4059,7 +4074,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83">
+      <c r="A83" s="3">
         <v>967129741</v>
       </c>
       <c r="B83" t="s">
@@ -4090,8 +4105,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A84">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
         <v>1286645029</v>
       </c>
       <c r="B84" t="s">
@@ -4122,8 +4137,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A85">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
         <v>745204575</v>
       </c>
       <c r="B85" t="s">
@@ -4154,8 +4169,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A86">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
         <v>1202771170</v>
       </c>
       <c r="B86" t="s">
@@ -4187,8 +4202,8 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87">
-        <v>755590360</v>
+      <c r="A87" s="3" t="s">
+        <v>346</v>
       </c>
       <c r="B87" t="s">
         <v>90</v>
@@ -4219,7 +4234,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88">
+      <c r="A88" s="3">
         <v>1356430970</v>
       </c>
       <c r="B88" t="s">
@@ -4251,7 +4266,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89">
+      <c r="A89" s="3">
         <v>1240383572</v>
       </c>
       <c r="B89" t="s">
@@ -4283,8 +4298,8 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <v>706191558</v>
+      <c r="A90" s="3" t="s">
+        <v>343</v>
       </c>
       <c r="B90" t="s">
         <v>93</v>
@@ -4315,7 +4330,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91">
+      <c r="A91" s="3">
         <v>928062579</v>
       </c>
       <c r="B91" t="s">
@@ -4347,7 +4362,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92">
+      <c r="A92" s="3">
         <v>925710253</v>
       </c>
       <c r="B92" t="s">
@@ -4378,8 +4393,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A93">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
         <v>923361238</v>
       </c>
       <c r="B93" t="s">
@@ -4411,7 +4426,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A94">
+      <c r="A94" s="3">
         <v>2461553211</v>
       </c>
       <c r="B94" t="s">
@@ -4442,8 +4457,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A95">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
         <v>1228266908</v>
       </c>
       <c r="B95" t="s">
@@ -4475,7 +4490,7 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96">
+      <c r="A96" s="3">
         <v>916711230</v>
       </c>
       <c r="B96" t="s">
@@ -4507,7 +4522,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97">
+      <c r="A97" s="3">
         <v>756505395</v>
       </c>
       <c r="B97" t="s">
@@ -4539,7 +4554,7 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98">
+      <c r="A98" s="3">
         <v>761061564</v>
       </c>
       <c r="B98" t="s">
@@ -4570,8 +4585,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A99">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
         <v>1378425171</v>
       </c>
       <c r="B99" t="s">
@@ -4602,8 +4617,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A100">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="3">
         <v>2418631102</v>
       </c>
       <c r="B100" t="s">
@@ -4635,7 +4650,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A101">
+      <c r="A101" s="3">
         <v>1218887438</v>
       </c>
       <c r="B101" t="s">
@@ -4666,8 +4681,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A102">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="3">
         <v>719922891</v>
       </c>
       <c r="B102" t="s">
@@ -4699,7 +4714,7 @@
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A103">
+      <c r="A103" s="3">
         <v>1225454895</v>
       </c>
       <c r="B103" t="s">
@@ -4731,7 +4746,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A104">
+      <c r="A104" s="3">
         <v>908109770</v>
       </c>
       <c r="B104" t="s">
@@ -4763,7 +4778,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A105">
+      <c r="A105" s="3">
         <v>1206923219</v>
       </c>
       <c r="B105" t="s">
@@ -4795,7 +4810,7 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106">
+      <c r="A106" s="3">
         <v>1234567890</v>
       </c>
       <c r="B106" t="s">
@@ -4827,7 +4842,7 @@
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107">
+      <c r="A107" s="3">
         <v>917406837</v>
       </c>
       <c r="B107" t="s">
@@ -4859,13 +4874,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J107" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Software"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se modularizo evaluacion y se añadieron skeletons
</commit_message>
<xml_diff>
--- a/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
+++ b/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSelectAI\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B3D89A-04BC-4278-8B57-2868C6988B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCBE592-39FB-4784-B9D9-19F98E79EA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="351">
   <si>
     <t>Cedula</t>
   </si>
@@ -1064,13 +1064,25 @@
   </si>
   <si>
     <t>0755590360</t>
+  </si>
+  <si>
+    <t>2300371198</t>
+  </si>
+  <si>
+    <t>Joffre Jhoel</t>
+  </si>
+  <si>
+    <t>Basurto Orejuela</t>
+  </si>
+  <si>
+    <t>jbasurtoo@unemi.edu.ec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1082,6 +1094,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1119,10 +1139,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1131,8 +1152,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1435,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4873,7 +4896,42 @@
         <v>340</v>
       </c>
     </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B108" t="s">
+        <v>348</v>
+      </c>
+      <c r="C108" t="s">
+        <v>349</v>
+      </c>
+      <c r="D108" t="s">
+        <v>210</v>
+      </c>
+      <c r="E108">
+        <v>7</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="G108" t="s">
+        <v>323</v>
+      </c>
+      <c r="H108" t="s">
+        <v>337</v>
+      </c>
+      <c r="I108" t="s">
+        <v>338</v>
+      </c>
+      <c r="J108" t="s">
+        <v>340</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F108" r:id="rId1" xr:uid="{694B8122-7596-4E2F-B990-CC0F98F9D9B2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adelanto de Fechas de Postulacion
</commit_message>
<xml_diff>
--- a/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
+++ b/backend/uploads/Estudiantes_UNEMI_Rol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSelectAI\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCBE592-39FB-4784-B9D9-19F98E79EA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D116C1C-DDA5-47F1-8D8E-252AE3F3F1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1460,14 +1460,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="J110" sqref="J110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4381,7 +4381,7 @@
         <v>338</v>
       </c>
       <c r="J91" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
@@ -4413,7 +4413,7 @@
         <v>338</v>
       </c>
       <c r="J92" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -4826,10 +4826,10 @@
         <v>326</v>
       </c>
       <c r="I105" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J105" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>